<commit_message>
final upload of work
</commit_message>
<xml_diff>
--- a/Execution_time_energy_Consump_Results_4GB.xlsx
+++ b/Execution_time_energy_Consump_Results_4GB.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spachava\Downloads\INRAE_M2_Stage_Work_April_August_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C02DA13-F2C3-456C-92B4-B4AE52055AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C2BED0-EF99-46E6-BA8A-0CA279C9C042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{7026C45D-988B-4980-9D6F-9E9655D0F0CD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{7026C45D-988B-4980-9D6F-9E9655D0F0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="136">
   <si>
     <t>52 914 mWh</t>
   </si>
@@ -424,13 +425,31 @@
   </si>
   <si>
     <t>4GB - cebanewdata</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>2.5 GB</t>
+  </si>
+  <si>
+    <t>4.5 GB</t>
+  </si>
+  <si>
+    <t>% of optimization for each workload</t>
+  </si>
+  <si>
+    <t>DB Size</t>
+  </si>
+  <si>
+    <t>Parameter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -454,8 +473,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -510,6 +536,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -523,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -544,13 +582,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -566,6 +598,45 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -882,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B97D693-E757-47FA-8F34-9FD888F40BEA}">
   <dimension ref="A1:L123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="H114" sqref="H114"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99:D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -892,8 +963,8 @@
     <col min="7" max="7" width="17.36328125" customWidth="1"/>
     <col min="8" max="8" width="12.453125" customWidth="1"/>
     <col min="9" max="9" width="12.81640625" customWidth="1"/>
-    <col min="10" max="10" width="15.90625" customWidth="1"/>
-    <col min="11" max="11" width="15.453125" customWidth="1"/>
+    <col min="10" max="10" width="13.90625" customWidth="1"/>
+    <col min="11" max="11" width="21.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -946,10 +1017,10 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="15">
         <v>284.86</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="15">
         <v>14.24</v>
       </c>
       <c r="D3">
@@ -975,8 +1046,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
       <c r="E4" t="s">
         <v>12</v>
       </c>
@@ -988,10 +1059,10 @@
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="15">
         <v>271.77999999999997</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="15">
         <v>13.59</v>
       </c>
       <c r="D5">
@@ -1017,8 +1088,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
       <c r="E6" t="s">
         <v>29</v>
       </c>
@@ -1030,10 +1101,10 @@
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="15">
         <v>297.58999999999997</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="15">
         <v>14.89</v>
       </c>
       <c r="D7">
@@ -1059,8 +1130,8 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
       <c r="E8" t="s">
         <v>31</v>
       </c>
@@ -1072,10 +1143,10 @@
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="15">
         <v>242.58</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="15">
         <v>12.13</v>
       </c>
       <c r="D9">
@@ -1101,8 +1172,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
       <c r="E10" t="s">
         <v>98</v>
       </c>
@@ -1114,10 +1185,10 @@
       <c r="A11">
         <v>5</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="15">
         <v>242.17</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="15">
         <v>12.12</v>
       </c>
       <c r="D11">
@@ -1546,7 +1617,7 @@
       <c r="J31" s="2">
         <v>74.3</v>
       </c>
-      <c r="K31" s="19">
+      <c r="K31" s="17">
         <v>2273</v>
       </c>
     </row>
@@ -1875,7 +1946,7 @@
       <c r="J49" s="2">
         <v>47.98</v>
       </c>
-      <c r="K49" s="19">
+      <c r="K49" s="17">
         <v>1420</v>
       </c>
     </row>
@@ -2351,7 +2422,7 @@
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A77" s="18">
+      <c r="A77" s="16">
         <v>6</v>
       </c>
       <c r="B77" s="8" t="s">
@@ -2609,7 +2680,7 @@
         <v>1783.4</v>
       </c>
     </row>
-    <row r="115" spans="6:11" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="6:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F115" s="9" t="s">
         <v>99</v>
       </c>
@@ -2618,7 +2689,7 @@
       <c r="I115" s="10"/>
       <c r="J115" s="10"/>
     </row>
-    <row r="116" spans="6:11" ht="31" x14ac:dyDescent="0.35">
+    <row r="116" spans="6:11" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F116" s="11" t="s">
         <v>100</v>
       </c>
@@ -2639,87 +2710,87 @@
       </c>
     </row>
     <row r="117" spans="6:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F117" s="12" t="s">
+      <c r="F117" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="G117" s="13" t="s">
+      <c r="G117" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="H117" s="13" t="s">
+      <c r="H117" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="I117" s="13" t="s">
+      <c r="I117" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="J117" s="13" t="s">
+      <c r="J117" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="K117" s="13" t="s">
+      <c r="K117" s="20" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="118" spans="6:11" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F118" s="12" t="s">
+      <c r="F118" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="G118" s="13" t="s">
+      <c r="G118" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="H118" s="13" t="s">
+      <c r="H118" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="I118" s="13" t="s">
+      <c r="I118" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="J118" s="13" t="s">
+      <c r="J118" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="K118" s="13" t="s">
+      <c r="K118" s="20" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="119" spans="6:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F119" s="12" t="s">
+      <c r="F119" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="G119" s="13" t="s">
+      <c r="G119" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="H119" s="13" t="s">
+      <c r="H119" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="I119" s="13" t="s">
+      <c r="I119" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="J119" s="13" t="s">
+      <c r="J119" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="K119" s="13" t="s">
+      <c r="K119" s="20" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="120" spans="6:11" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F120" s="14" t="s">
+    <row r="120" spans="6:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F120" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="G120" s="15" t="s">
+      <c r="G120" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="H120" s="15" t="s">
+      <c r="H120" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="I120" s="15" t="s">
+      <c r="I120" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="J120" s="15" t="s">
+      <c r="J120" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="K120" s="15" t="s">
+      <c r="K120" s="21" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="121" spans="6:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F121" s="16" t="s">
+      <c r="F121" s="14" t="s">
         <v>109</v>
       </c>
       <c r="G121" s="10"/>
@@ -2728,7 +2799,7 @@
       <c r="J121" s="10"/>
       <c r="K121" s="10"/>
     </row>
-    <row r="122" spans="6:11" ht="31" x14ac:dyDescent="0.35">
+    <row r="122" spans="6:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F122" s="11" t="s">
         <v>100</v>
       </c>
@@ -2742,29 +2813,29 @@
         <v>103</v>
       </c>
       <c r="J122" s="11" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="K122" s="11" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="123" spans="6:11" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F123" s="12" t="s">
+      <c r="F123" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="G123" s="13" t="s">
+      <c r="G123" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="H123" s="13" t="s">
+      <c r="H123" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="I123" s="13" t="s">
+      <c r="I123" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="J123" s="13" t="s">
+      <c r="J123" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="K123" s="13" t="s">
+      <c r="K123" s="20" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2772,4 +2843,130 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABBBDA04-4917-4D80-9E83-20DF1F7C42BC}">
+  <dimension ref="D7:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="12.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="4:8" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+    </row>
+    <row r="8" spans="4:8" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" s="27">
+        <v>1.6799999999999999E-2</v>
+      </c>
+      <c r="G9" s="25">
+        <v>0.1429</v>
+      </c>
+      <c r="H9" s="26">
+        <v>-3.8699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="24"/>
+      <c r="E10" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10" s="27">
+        <v>4.1399999999999999E-2</v>
+      </c>
+      <c r="G10" s="25">
+        <v>0.1188</v>
+      </c>
+      <c r="H10" s="26">
+        <v>-0.2298</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+    </row>
+    <row r="12" spans="4:8" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="F12" s="25">
+        <v>0.1555</v>
+      </c>
+      <c r="G12" s="27">
+        <v>4.7800000000000002E-2</v>
+      </c>
+      <c r="H12" s="26">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="4:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="24"/>
+      <c r="E13" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F13" s="25">
+        <v>6.13E-2</v>
+      </c>
+      <c r="G13" s="27">
+        <v>1.41E-2</v>
+      </c>
+      <c r="H13" s="26">
+        <v>-0.23799999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D11:H11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>